<commit_message>
adding parentId in sawarmo
</commit_message>
<xml_diff>
--- a/server/data/mainData.xlsx
+++ b/server/data/mainData.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C46AA1-9CCB-5E41-9E28-AE045C193743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="735" windowWidth="30240" windowHeight="18900"/>
   </bookViews>
   <sheets>
     <sheet name="Main_Table" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="40">
   <si>
     <t>SID</t>
   </si>
@@ -159,19 +158,13 @@
     <t>i</t>
   </si>
   <si>
-    <t>მიზეზი</t>
-  </si>
-  <si>
-    <t>Reject_Reason</t>
-  </si>
-  <si>
-    <t>n/a</t>
+    <t>ParentId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -240,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -258,7 +251,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,591 +530,591 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="AD6" sqref="AD6"/>
+    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="6" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" customWidth="1"/>
-    <col min="12" max="13" width="10.1640625" customWidth="1"/>
-    <col min="16" max="16" width="14.1640625" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" customWidth="1"/>
-    <col min="18" max="18" width="12" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="7" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="13" max="14" width="10.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>40</v>
-      </c>
     </row>
-    <row r="2" spans="1:26" ht="56" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>16063451</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>150011008</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>2</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>591940994</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="2">
+      <c r="Q2" s="2">
         <v>577111941</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="2">
+      <c r="S2" s="2">
         <v>591940994</v>
       </c>
-      <c r="S2" s="2">
+      <c r="T2" s="2">
         <v>130</v>
       </c>
-      <c r="T2" s="2">
+      <c r="U2" s="2">
         <v>1</v>
       </c>
-      <c r="U2" s="2">
+      <c r="V2" s="2">
         <v>2</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="X2" s="6">
+      <c r="Y2" s="6">
         <v>0</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>1</v>
       </c>
-      <c r="Z2" s="7" t="s">
-        <v>41</v>
-      </c>
     </row>
-    <row r="3" spans="1:26" ht="56" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="51" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>17063451</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>150011008</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>2</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>591940994</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="2">
+      <c r="Q3" s="2">
         <v>577111941</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="2">
+      <c r="S3" s="2">
         <v>591940994</v>
       </c>
-      <c r="S3" s="2">
+      <c r="T3" s="2">
         <v>130</v>
       </c>
-      <c r="T3" s="2">
+      <c r="U3" s="2">
         <v>2</v>
       </c>
-      <c r="U3" s="2">
+      <c r="V3" s="2">
         <v>1</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="X3" s="6">
+      <c r="Y3" s="6">
         <v>0</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>1</v>
       </c>
-      <c r="Z3" s="7" t="s">
-        <v>41</v>
-      </c>
     </row>
-    <row r="4" spans="1:26" ht="56" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>18063451</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>150011008</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>2</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>591940994</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="2">
+      <c r="Q4" s="2">
         <v>577111941</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R4" s="2">
+      <c r="S4" s="2">
         <v>591940994</v>
       </c>
-      <c r="S4" s="2">
+      <c r="T4" s="2">
         <v>130</v>
       </c>
-      <c r="T4" s="2">
+      <c r="U4" s="2">
         <v>3</v>
       </c>
-      <c r="U4" s="2">
+      <c r="V4" s="2">
         <v>2</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="X4" s="6">
+      <c r="Y4" s="6">
         <v>0</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>1</v>
       </c>
-      <c r="Z4" s="7" t="s">
-        <v>41</v>
-      </c>
     </row>
-    <row r="5" spans="1:26" ht="56" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="51" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>19063451</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>150011008</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>2</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>591940994</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P5" s="2">
+      <c r="Q5" s="2">
         <v>577111941</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="R5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R5" s="2">
+      <c r="S5" s="2">
         <v>591940994</v>
       </c>
-      <c r="S5" s="2">
+      <c r="T5" s="2">
         <v>130</v>
       </c>
-      <c r="T5" s="2">
+      <c r="U5" s="2">
         <v>1</v>
       </c>
-      <c r="U5" s="2">
+      <c r="V5" s="2">
         <v>2</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="W5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="X5" s="6">
+      <c r="Y5" s="6">
         <v>4</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>1</v>
       </c>
-      <c r="Z5" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="6" spans="1:26" ht="56" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="51" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>20063451</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>150011008</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>2</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>591940994</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="2">
+      <c r="Q6" s="2">
         <v>577111941</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="R6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R6" s="2">
+      <c r="S6" s="2">
         <v>591940994</v>
       </c>
-      <c r="S6" s="2">
+      <c r="T6" s="2">
         <v>130</v>
       </c>
-      <c r="T6" s="2">
+      <c r="U6" s="2">
         <v>2</v>
       </c>
-      <c r="U6" s="2">
+      <c r="V6" s="2">
         <v>1</v>
       </c>
-      <c r="V6" s="2" t="s">
+      <c r="W6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="W6" s="2" t="s">
+      <c r="X6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="X6" s="6">
+      <c r="Y6" s="6">
         <v>0</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>1</v>
       </c>
-      <c r="Z6" s="7" t="s">
-        <v>41</v>
-      </c>
     </row>
-    <row r="7" spans="1:26" ht="56" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="51" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>21063451</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>150011008</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>2</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>591940994</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P7" s="2">
+      <c r="Q7" s="2">
         <v>577111941</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R7" s="2">
+      <c r="S7" s="2">
         <v>591940994</v>
       </c>
-      <c r="S7" s="2">
+      <c r="T7" s="2">
         <v>130</v>
       </c>
-      <c r="T7" s="2">
+      <c r="U7" s="2">
         <v>3</v>
       </c>
-      <c r="U7" s="2">
+      <c r="V7" s="2">
         <v>2</v>
       </c>
-      <c r="V7" s="2" t="s">
+      <c r="W7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="X7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="X7" s="6">
+      <c r="Y7" s="6">
         <v>0</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>1</v>
       </c>
-      <c r="Z7" s="7" t="s">
-        <v>41</v>
-      </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -1131,9 +1123,9 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="5"/>
+      <c r="L8" s="4"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="4"/>
+      <c r="N8" s="5"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
@@ -1143,13 +1135,14 @@
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
-      <c r="X8" s="6"/>
+      <c r="X8" s="4"/>
       <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -1158,9 +1151,9 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="5"/>
+      <c r="L9" s="4"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="4"/>
+      <c r="N9" s="5"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
@@ -1170,13 +1163,14 @@
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
-      <c r="X9" s="6"/>
+      <c r="X9" s="4"/>
       <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -1185,9 +1179,9 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-      <c r="L10" s="5"/>
+      <c r="L10" s="4"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="4"/>
+      <c r="N10" s="5"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
@@ -1197,13 +1191,14 @@
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
-      <c r="X10" s="6"/>
+      <c r="X10" s="4"/>
       <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -1212,9 +1207,9 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="5"/>
+      <c r="L11" s="4"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="4"/>
+      <c r="N11" s="5"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
@@ -1224,13 +1219,14 @@
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
-      <c r="X11" s="6"/>
+      <c r="X11" s="4"/>
       <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -1239,9 +1235,9 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="5"/>
+      <c r="L12" s="4"/>
       <c r="M12" s="5"/>
-      <c r="N12" s="4"/>
+      <c r="N12" s="5"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
@@ -1251,8 +1247,9 @@
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
-      <c r="X12" s="6"/>
+      <c r="X12" s="4"/>
       <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding filter in data
</commit_message>
<xml_diff>
--- a/server/data/mainData.xlsx
+++ b/server/data/mainData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="46">
   <si>
     <t>SID</t>
   </si>
@@ -159,6 +159,24 @@
   </si>
   <si>
     <t>ParentId</t>
+  </si>
+  <si>
+    <t>12 11 13 11</t>
+  </si>
+  <si>
+    <t>16 11 13 11</t>
+  </si>
+  <si>
+    <t>18 11 13 11</t>
+  </si>
+  <si>
+    <t>20 11 13 11</t>
+  </si>
+  <si>
+    <t>19 11 13 11</t>
+  </si>
+  <si>
+    <t>areaCode</t>
   </si>
 </sst>
 </file>
@@ -531,27 +549,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:AA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="105" workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="7" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" customWidth="1"/>
-    <col min="13" max="14" width="10.140625" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" customWidth="1"/>
-    <col min="19" max="19" width="12" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="8" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="14" max="15" width="10.140625" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,73 +583,76 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>16063451</v>
       </c>
@@ -644,74 +665,77 @@
       <c r="D2" s="2">
         <v>150011008</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="2">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="2">
-        <v>2</v>
-      </c>
       <c r="L2" s="2">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2">
         <v>591940994</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="R2" s="2">
         <v>577111941</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S2" s="2">
+      <c r="T2" s="2">
         <v>591940994</v>
       </c>
-      <c r="T2" s="2">
+      <c r="U2" s="2">
         <v>130</v>
       </c>
-      <c r="U2" s="2">
+      <c r="V2" s="2">
         <v>1</v>
       </c>
-      <c r="V2" s="2">
-        <v>2</v>
-      </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" s="2">
+        <v>2</v>
+      </c>
+      <c r="X2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Y2" s="6">
+      <c r="Z2" s="6">
         <v>0</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="51" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>17063451</v>
       </c>
@@ -724,74 +748,77 @@
       <c r="D3" s="2">
         <v>150011008</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>27</v>
+      <c r="E3" s="2">
+        <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="2">
-        <v>2</v>
-      </c>
       <c r="L3" s="2">
+        <v>2</v>
+      </c>
+      <c r="M3" s="2">
         <v>591940994</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="R3" s="2">
         <v>577111941</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="2">
+      <c r="T3" s="2">
         <v>591940994</v>
       </c>
-      <c r="T3" s="2">
+      <c r="U3" s="2">
         <v>130</v>
       </c>
-      <c r="U3" s="2">
-        <v>2</v>
-      </c>
       <c r="V3" s="2">
+        <v>2</v>
+      </c>
+      <c r="W3" s="2">
         <v>1</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Y3" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z3">
+      <c r="Z3" s="6">
         <v>1</v>
       </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" ht="51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>18063451</v>
       </c>
@@ -804,74 +831,77 @@
       <c r="D4" s="2">
         <v>150011008</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>27</v>
+      <c r="E4" s="2">
+        <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="2">
-        <v>2</v>
-      </c>
       <c r="L4" s="2">
+        <v>2</v>
+      </c>
+      <c r="M4" s="2">
         <v>591940994</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="R4" s="2">
         <v>577111941</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S4" s="2">
+      <c r="T4" s="2">
         <v>591940994</v>
       </c>
-      <c r="T4" s="2">
+      <c r="U4" s="2">
         <v>130</v>
       </c>
-      <c r="U4" s="2">
+      <c r="V4" s="2">
         <v>3</v>
       </c>
-      <c r="V4" s="2">
-        <v>2</v>
-      </c>
-      <c r="W4" s="2" t="s">
+      <c r="W4" s="2">
+        <v>2</v>
+      </c>
+      <c r="X4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="X4" s="2" t="s">
+      <c r="Y4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Y4" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z4">
+      <c r="Z4" s="6">
+        <v>2</v>
+      </c>
+      <c r="AA4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="51" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>19063451</v>
       </c>
@@ -884,74 +914,77 @@
       <c r="D5" s="2">
         <v>150011008</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>27</v>
+      <c r="E5" s="2">
+        <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="2">
-        <v>2</v>
-      </c>
       <c r="L5" s="2">
+        <v>2</v>
+      </c>
+      <c r="M5" s="2">
         <v>591940994</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="R5" s="2">
         <v>577111941</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S5" s="2">
+      <c r="T5" s="2">
         <v>591940994</v>
       </c>
-      <c r="T5" s="2">
+      <c r="U5" s="2">
         <v>130</v>
       </c>
-      <c r="U5" s="2">
+      <c r="V5" s="2">
         <v>1</v>
       </c>
-      <c r="V5" s="2">
-        <v>2</v>
-      </c>
-      <c r="W5" s="2" t="s">
+      <c r="W5" s="2">
+        <v>2</v>
+      </c>
+      <c r="X5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="X5" s="2" t="s">
+      <c r="Y5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Y5" s="6">
+      <c r="Z5" s="6">
         <v>4</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="51" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>20063451</v>
       </c>
@@ -964,74 +997,77 @@
       <c r="D6" s="2">
         <v>150011008</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>27</v>
+      <c r="E6" s="2">
+        <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="2">
-        <v>2</v>
-      </c>
       <c r="L6" s="2">
+        <v>2</v>
+      </c>
+      <c r="M6" s="2">
         <v>591940994</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="R6" s="2">
         <v>577111941</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="S6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S6" s="2">
+      <c r="T6" s="2">
         <v>591940994</v>
       </c>
-      <c r="T6" s="2">
+      <c r="U6" s="2">
         <v>130</v>
       </c>
-      <c r="U6" s="2">
-        <v>2</v>
-      </c>
       <c r="V6" s="2">
+        <v>2</v>
+      </c>
+      <c r="W6" s="2">
         <v>1</v>
       </c>
-      <c r="W6" s="2" t="s">
+      <c r="X6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="X6" s="2" t="s">
+      <c r="Y6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Y6" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
+      <c r="Z6" s="6">
+        <v>2</v>
+      </c>
+      <c r="AA6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="51" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>21063451</v>
       </c>
@@ -1044,74 +1080,77 @@
       <c r="D7" s="2">
         <v>150011008</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>27</v>
+      <c r="E7" s="2">
+        <v>20</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="2">
-        <v>2</v>
-      </c>
       <c r="L7" s="2">
+        <v>2</v>
+      </c>
+      <c r="M7" s="2">
         <v>591940994</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="R7" s="2">
         <v>577111941</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="S7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S7" s="2">
+      <c r="T7" s="2">
         <v>591940994</v>
       </c>
-      <c r="T7" s="2">
+      <c r="U7" s="2">
         <v>130</v>
       </c>
-      <c r="U7" s="2">
+      <c r="V7" s="2">
         <v>3</v>
       </c>
-      <c r="V7" s="2">
-        <v>2</v>
-      </c>
-      <c r="W7" s="2" t="s">
+      <c r="W7" s="2">
+        <v>2</v>
+      </c>
+      <c r="X7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="X7" s="2" t="s">
+      <c r="Y7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="Y7" s="6">
+      <c r="Z7" s="6">
         <v>0</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
@@ -1124,9 +1163,9 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="5"/>
+      <c r="M8" s="4"/>
       <c r="N8" s="5"/>
-      <c r="O8" s="4"/>
+      <c r="O8" s="5"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
@@ -1136,10 +1175,11 @@
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
-      <c r="Y8" s="6"/>
+      <c r="Y8" s="4"/>
       <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
@@ -1152,9 +1192,9 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="5"/>
+      <c r="M9" s="4"/>
       <c r="N9" s="5"/>
-      <c r="O9" s="4"/>
+      <c r="O9" s="5"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
@@ -1164,10 +1204,11 @@
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
-      <c r="Y9" s="6"/>
+      <c r="Y9" s="4"/>
       <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
@@ -1180,9 +1221,9 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="5"/>
+      <c r="M10" s="4"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="4"/>
+      <c r="O10" s="5"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
@@ -1192,10 +1233,11 @@
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
-      <c r="Y10" s="6"/>
+      <c r="Y10" s="4"/>
       <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
@@ -1208,9 +1250,9 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="5"/>
+      <c r="M11" s="4"/>
       <c r="N11" s="5"/>
-      <c r="O11" s="4"/>
+      <c r="O11" s="5"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
@@ -1220,10 +1262,11 @@
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
-      <c r="Y11" s="6"/>
+      <c r="Y11" s="4"/>
       <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
@@ -1236,9 +1279,9 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="5"/>
+      <c r="M12" s="4"/>
       <c r="N12" s="5"/>
-      <c r="O12" s="4"/>
+      <c r="O12" s="5"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
@@ -1248,8 +1291,9 @@
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
-      <c r="Y12" s="6"/>
+      <c r="Y12" s="4"/>
       <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>